<commit_message>
accessed mainController scope in search bar directive
</commit_message>
<xml_diff>
--- a/rentafail_1/data/url-id-extract.xlsx
+++ b/rentafail_1/data/url-id-extract.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>rqWgkXeBD4c</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=l-kxBjNML5c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheerleading Fail </t>
+  </si>
+  <si>
+    <t>"http://www.youtube.com/embed/l-kxBjNML5c?autoplay=0"</t>
   </si>
 </sst>
 </file>
@@ -417,24 +426,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -457,7 +466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -488,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -511,13 +520,37 @@
       </c>
       <c r="I3" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="str">
+        <f>D4&amp;MID(F4, 33, 20)&amp;$G$2</f>
+        <v>"http://www.youtube.com/embed/l-kxBjNML5c?autoplay=0"</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="str">
+        <f>MID(F4, 33, 20)</f>
+        <v>l-kxBjNML5c</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" display="http://www.youtube.com/embed/rqWgkXeBD4c?autoplay=0"/>
     <hyperlink ref="F3" r:id="rId2" display="https://www.youtube.com/watch?v=3lCm9Ii4L48"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>